<commit_message>
- Ajouté des fichiers à importer pour la région 7.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21196 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Région 7/id.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Région 7/id.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>_id</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Balcon du Jura</t>
+  </si>
+  <si>
+    <t>Mont-Aubert</t>
+  </si>
+  <si>
+    <t>Montagny – Champvent</t>
+  </si>
+  <si>
+    <t>Pâquier – Donneloye</t>
+  </si>
+  <si>
+    <t>Yvonand</t>
   </si>
 </sst>
 </file>
@@ -445,7 +457,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -478,7 +490,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>7010000000</v>
@@ -500,32 +512,96 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>7040000000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7040</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>7050000000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7050</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7060000000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7060</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>7100000000</v>
+      </c>
+      <c r="C6" s="5">
+        <v>7100</v>
+      </c>
+      <c r="D6" s="5">
+        <v>7000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>

</xml_diff>